<commit_message>
please review. ready for fall 21
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\radarinstructor\ECE-Radar-Project-Instructor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\radarproj\ECE-Radar-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="116">
   <si>
     <t>Col0</t>
   </si>
@@ -238,13 +238,220 @@
   </si>
   <si>
     <t>Table 7: RADAR Burn-Through Power-Range (km)</t>
+  </si>
+  <si>
+    <t>SAM Site Radio Intel:</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Gain</t>
+  </si>
+  <si>
+    <r>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>T</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>R</t>
+    </r>
+  </si>
+  <si>
+    <t>MPQ-26</t>
+  </si>
+  <si>
+    <t>60 MHz</t>
+  </si>
+  <si>
+    <t>50 W</t>
+  </si>
+  <si>
+    <t>1 nW</t>
+  </si>
+  <si>
+    <t>MPQ-30</t>
+  </si>
+  <si>
+    <t>MPQ-32</t>
+  </si>
+  <si>
+    <t>SAM Site Radar Intel:</t>
+  </si>
+  <si>
+    <r>
+      <t>SNR</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>req</t>
+    </r>
+  </si>
+  <si>
+    <t>4.5 GHz</t>
+  </si>
+  <si>
+    <t>8 kW</t>
+  </si>
+  <si>
+    <t>1 fW</t>
+  </si>
+  <si>
+    <t>9 kW</t>
+  </si>
+  <si>
+    <t>10 kW</t>
+  </si>
+  <si>
+    <t>Aircraft Package Options:</t>
+  </si>
+  <si>
+    <t>Composition</t>
+  </si>
+  <si>
+    <t>RCS</t>
+  </si>
+  <si>
+    <t>Altitude</t>
+  </si>
+  <si>
+    <t>HARM Capability</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Conventional Strike</t>
+  </si>
+  <si>
+    <t>1xEA-18G + 2xF-15E</t>
+  </si>
+  <si>
+    <r>
+      <t>5.5 m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>2000 ft</t>
+  </si>
+  <si>
+    <t>Mixed Strike</t>
+  </si>
+  <si>
+    <t>1xF-16CJ+2xF-35</t>
+  </si>
+  <si>
+    <r>
+      <t>3.5 m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>3000 ft</t>
+  </si>
+  <si>
+    <t>Stealth Strike</t>
+  </si>
+  <si>
+    <t>2xF-22</t>
+  </si>
+  <si>
+    <r>
+      <t>0.01 m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>6000 ft</t>
+  </si>
+  <si>
+    <t>Aircraft RWR Intel:</t>
+  </si>
+  <si>
+    <t>5 nW</t>
+  </si>
+  <si>
+    <t>Aircraft Jammer Intel:</t>
+  </si>
+  <si>
+    <t>10 W</t>
+  </si>
+  <si>
+    <t>8 W</t>
+  </si>
+  <si>
+    <t>5 W</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -259,6 +466,34 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="subscript"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -281,7 +516,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -814,11 +1049,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
@@ -952,6 +1211,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="4" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1292,13 +1564,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J120"/>
+  <dimension ref="A1:J132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F83" sqref="F83"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="G107" sqref="G107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.25" customWidth="1"/>
     <col min="2" max="4" width="11.5" customWidth="1"/>
@@ -1306,7 +1578,7 @@
     <col min="6" max="10" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1338,7 +1610,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1370,7 +1642,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -1402,7 +1674,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
@@ -1430,7 +1702,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -1478,7 +1750,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="44" t="s">
         <v>11</v>
       </c>
@@ -1510,7 +1782,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="47" t="s">
         <v>15</v>
       </c>
@@ -1542,7 +1814,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="47" t="s">
         <v>16</v>
       </c>
@@ -1606,7 +1878,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
@@ -1718,7 +1990,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="28" t="s">
         <v>25</v>
       </c>
@@ -1814,7 +2086,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="34" t="s">
         <v>25</v>
       </c>
@@ -1910,7 +2182,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="34" t="s">
         <v>25</v>
       </c>
@@ -2006,7 +2278,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="34" t="s">
         <v>25</v>
       </c>
@@ -2070,7 +2342,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>11</v>
       </c>
@@ -2138,7 +2410,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="47" t="s">
         <v>28</v>
       </c>
@@ -2170,7 +2442,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="47" t="s">
         <v>29</v>
       </c>
@@ -2202,7 +2474,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="47" t="s">
         <v>30</v>
       </c>
@@ -2266,7 +2538,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>11</v>
       </c>
@@ -2316,7 +2588,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="44" t="s">
         <v>11</v>
       </c>
@@ -2348,7 +2620,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="47" t="s">
         <v>15</v>
       </c>
@@ -2380,7 +2652,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="47" t="s">
         <v>16</v>
       </c>
@@ -2444,7 +2716,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>11</v>
       </c>
@@ -2498,7 +2770,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="44" t="s">
         <v>11</v>
       </c>
@@ -2530,7 +2802,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="47" t="s">
         <v>18</v>
       </c>
@@ -2562,7 +2834,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="47" t="s">
         <v>19</v>
       </c>
@@ -2594,7 +2866,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="47" t="s">
         <v>20</v>
       </c>
@@ -2626,7 +2898,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="47" t="s">
         <v>21</v>
       </c>
@@ -2690,7 +2962,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>11</v>
       </c>
@@ -2746,7 +3018,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="44" t="s">
         <v>11</v>
       </c>
@@ -2778,7 +3050,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="47" t="s">
         <v>36</v>
       </c>
@@ -2810,7 +3082,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="47" t="s">
         <v>37</v>
       </c>
@@ -2842,7 +3114,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="47" t="s">
         <v>38</v>
       </c>
@@ -2874,7 +3146,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="47" t="s">
         <v>39</v>
       </c>
@@ -2938,7 +3210,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>11</v>
       </c>
@@ -2996,7 +3268,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="44" t="s">
         <v>11</v>
       </c>
@@ -3028,7 +3300,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="47" t="s">
         <v>15</v>
       </c>
@@ -3060,7 +3332,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="47" t="s">
         <v>16</v>
       </c>
@@ -3124,7 +3396,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>11</v>
       </c>
@@ -3174,7 +3446,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="44" t="s">
         <v>11</v>
       </c>
@@ -3206,7 +3478,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="47" t="s">
         <v>15</v>
       </c>
@@ -3238,7 +3510,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="47" t="s">
         <v>16</v>
       </c>
@@ -3302,7 +3574,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>11</v>
       </c>
@@ -3352,7 +3624,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="44" t="s">
         <v>11</v>
       </c>
@@ -3384,7 +3656,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="47" t="s">
         <v>41</v>
       </c>
@@ -3416,7 +3688,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="47" t="s">
         <v>42</v>
       </c>
@@ -3448,7 +3720,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="47" t="s">
         <v>43</v>
       </c>
@@ -3480,7 +3752,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="47" t="s">
         <v>44</v>
       </c>
@@ -3512,7 +3784,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="47" t="s">
         <v>45</v>
       </c>
@@ -3544,7 +3816,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="47" t="s">
         <v>46</v>
       </c>
@@ -3576,7 +3848,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="47" t="s">
         <v>47</v>
       </c>
@@ -3608,7 +3880,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="47" t="s">
         <v>48</v>
       </c>
@@ -3640,7 +3912,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="47" t="s">
         <v>49</v>
       </c>
@@ -3672,7 +3944,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="47" t="s">
         <v>49</v>
       </c>
@@ -3704,7 +3976,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="47" t="s">
         <v>48</v>
       </c>
@@ -3736,7 +4008,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="47" t="s">
         <v>47</v>
       </c>
@@ -3768,7 +4040,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="47" t="s">
         <v>46</v>
       </c>
@@ -3800,7 +4072,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="47" t="s">
         <v>45</v>
       </c>
@@ -3832,7 +4104,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="47" t="s">
         <v>44</v>
       </c>
@@ -3864,7 +4136,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="47" t="s">
         <v>43</v>
       </c>
@@ -3896,7 +4168,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="47" t="s">
         <v>42</v>
       </c>
@@ -3960,7 +4232,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>11</v>
       </c>
@@ -4006,7 +4278,7 @@
       <c r="I89" s="3"/>
       <c r="J89" s="3"/>
     </row>
-    <row r="90" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="44" t="s">
         <v>51</v>
       </c>
@@ -4036,7 +4308,7 @@
       </c>
       <c r="J90" s="3"/>
     </row>
-    <row r="91" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="47" t="s">
         <v>53</v>
       </c>
@@ -4068,7 +4340,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="47" t="s">
         <v>54</v>
       </c>
@@ -4100,7 +4372,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="47" t="s">
         <v>55</v>
       </c>
@@ -4164,7 +4436,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="95" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>11</v>
       </c>
@@ -4210,7 +4482,7 @@
       <c r="I96" s="3"/>
       <c r="J96" s="3"/>
     </row>
-    <row r="97" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="44" t="s">
         <v>58</v>
       </c>
@@ -4242,7 +4514,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="47" t="s">
         <v>59</v>
       </c>
@@ -4274,7 +4546,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="47" t="s">
         <v>60</v>
       </c>
@@ -4338,7 +4610,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>11</v>
       </c>
@@ -4370,7 +4642,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>11</v>
       </c>
@@ -4402,7 +4674,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>11</v>
       </c>
@@ -4434,28 +4706,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="104" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>11</v>
       </c>
-      <c r="B104" t="s">
-        <v>11</v>
-      </c>
-      <c r="C104" t="s">
-        <v>11</v>
-      </c>
-      <c r="D104" t="s">
-        <v>11</v>
-      </c>
-      <c r="E104" t="s">
-        <v>11</v>
-      </c>
-      <c r="F104" t="s">
-        <v>11</v>
-      </c>
-      <c r="G104" t="s">
-        <v>11</v>
-      </c>
+      <c r="B104" s="60" t="s">
+        <v>73</v>
+      </c>
+      <c r="C104" s="61"/>
+      <c r="D104" s="61"/>
+      <c r="E104" s="61"/>
+      <c r="F104" s="61"/>
       <c r="H104" t="s">
         <v>11</v>
       </c>
@@ -4466,27 +4727,24 @@
         <v>11</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>11</v>
       </c>
-      <c r="B105" t="s">
-        <v>11</v>
-      </c>
-      <c r="C105" t="s">
-        <v>11</v>
-      </c>
-      <c r="D105" t="s">
-        <v>11</v>
-      </c>
-      <c r="E105" t="s">
-        <v>11</v>
-      </c>
-      <c r="F105" t="s">
-        <v>11</v>
-      </c>
-      <c r="G105" t="s">
-        <v>11</v>
+      <c r="B105" s="58" t="s">
+        <v>74</v>
+      </c>
+      <c r="C105" s="58" t="s">
+        <v>75</v>
+      </c>
+      <c r="D105" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="E105" s="58" t="s">
+        <v>77</v>
+      </c>
+      <c r="F105" s="58" t="s">
+        <v>78</v>
       </c>
       <c r="H105" t="s">
         <v>11</v>
@@ -4498,27 +4756,24 @@
         <v>11</v>
       </c>
     </row>
-    <row r="106" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>11</v>
       </c>
-      <c r="B106" t="s">
-        <v>11</v>
-      </c>
-      <c r="C106" t="s">
-        <v>11</v>
-      </c>
-      <c r="D106" t="s">
-        <v>11</v>
-      </c>
-      <c r="E106" t="s">
-        <v>11</v>
-      </c>
-      <c r="F106" t="s">
-        <v>11</v>
-      </c>
-      <c r="G106" t="s">
-        <v>11</v>
+      <c r="B106" s="59" t="s">
+        <v>79</v>
+      </c>
+      <c r="C106" s="59" t="s">
+        <v>80</v>
+      </c>
+      <c r="D106" s="59">
+        <v>2</v>
+      </c>
+      <c r="E106" s="59" t="s">
+        <v>81</v>
+      </c>
+      <c r="F106" s="59" t="s">
+        <v>82</v>
       </c>
       <c r="H106" t="s">
         <v>11</v>
@@ -4530,27 +4785,24 @@
         <v>11</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>11</v>
       </c>
-      <c r="B107" t="s">
-        <v>11</v>
-      </c>
-      <c r="C107" t="s">
-        <v>11</v>
-      </c>
-      <c r="D107" t="s">
-        <v>11</v>
-      </c>
-      <c r="E107" t="s">
-        <v>11</v>
-      </c>
-      <c r="F107" t="s">
-        <v>11</v>
-      </c>
-      <c r="G107" t="s">
-        <v>11</v>
+      <c r="B107" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="C107" s="59" t="s">
+        <v>80</v>
+      </c>
+      <c r="D107" s="59">
+        <v>9</v>
+      </c>
+      <c r="E107" s="59" t="s">
+        <v>81</v>
+      </c>
+      <c r="F107" s="59" t="s">
+        <v>82</v>
       </c>
       <c r="H107" t="s">
         <v>11</v>
@@ -4562,27 +4814,24 @@
         <v>11</v>
       </c>
     </row>
-    <row r="108" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>11</v>
       </c>
-      <c r="B108" t="s">
-        <v>11</v>
-      </c>
-      <c r="C108" t="s">
-        <v>11</v>
-      </c>
-      <c r="D108" t="s">
-        <v>11</v>
-      </c>
-      <c r="E108" t="s">
-        <v>11</v>
-      </c>
-      <c r="F108" t="s">
-        <v>11</v>
-      </c>
-      <c r="G108" t="s">
-        <v>11</v>
+      <c r="B108" s="59" t="s">
+        <v>84</v>
+      </c>
+      <c r="C108" s="59" t="s">
+        <v>80</v>
+      </c>
+      <c r="D108" s="59">
+        <v>16</v>
+      </c>
+      <c r="E108" s="59" t="s">
+        <v>81</v>
+      </c>
+      <c r="F108" s="59" t="s">
+        <v>82</v>
       </c>
       <c r="H108" t="s">
         <v>11</v>
@@ -4594,28 +4843,10 @@
         <v>11</v>
       </c>
     </row>
-    <row r="109" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>11</v>
       </c>
-      <c r="B109" t="s">
-        <v>11</v>
-      </c>
-      <c r="C109" t="s">
-        <v>11</v>
-      </c>
-      <c r="D109" t="s">
-        <v>11</v>
-      </c>
-      <c r="E109" t="s">
-        <v>11</v>
-      </c>
-      <c r="F109" t="s">
-        <v>11</v>
-      </c>
-      <c r="G109" t="s">
-        <v>11</v>
-      </c>
       <c r="H109" t="s">
         <v>11</v>
       </c>
@@ -4626,28 +4857,18 @@
         <v>11</v>
       </c>
     </row>
-    <row r="110" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>11</v>
       </c>
-      <c r="B110" t="s">
-        <v>11</v>
-      </c>
-      <c r="C110" t="s">
-        <v>11</v>
-      </c>
-      <c r="D110" t="s">
-        <v>11</v>
-      </c>
-      <c r="E110" t="s">
-        <v>11</v>
-      </c>
-      <c r="F110" t="s">
-        <v>11</v>
-      </c>
-      <c r="G110" t="s">
-        <v>11</v>
-      </c>
+      <c r="B110" s="60" t="s">
+        <v>85</v>
+      </c>
+      <c r="C110" s="61"/>
+      <c r="D110" s="61"/>
+      <c r="E110" s="61"/>
+      <c r="F110" s="61"/>
+      <c r="G110" s="61"/>
       <c r="H110" t="s">
         <v>11</v>
       </c>
@@ -4658,27 +4879,27 @@
         <v>11</v>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>11</v>
       </c>
-      <c r="B111" t="s">
-        <v>11</v>
-      </c>
-      <c r="C111" t="s">
-        <v>11</v>
-      </c>
-      <c r="D111" t="s">
-        <v>11</v>
-      </c>
-      <c r="E111" t="s">
-        <v>11</v>
-      </c>
-      <c r="F111" t="s">
-        <v>11</v>
-      </c>
-      <c r="G111" t="s">
-        <v>11</v>
+      <c r="B111" s="58" t="s">
+        <v>74</v>
+      </c>
+      <c r="C111" s="58" t="s">
+        <v>75</v>
+      </c>
+      <c r="D111" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="E111" s="58" t="s">
+        <v>77</v>
+      </c>
+      <c r="F111" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="G111" s="58" t="s">
+        <v>86</v>
       </c>
       <c r="H111" t="s">
         <v>11</v>
@@ -4690,27 +4911,27 @@
         <v>11</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>11</v>
       </c>
-      <c r="B112" t="s">
-        <v>11</v>
-      </c>
-      <c r="C112" t="s">
-        <v>11</v>
-      </c>
-      <c r="D112" t="s">
-        <v>11</v>
-      </c>
-      <c r="E112" t="s">
-        <v>11</v>
-      </c>
-      <c r="F112" t="s">
-        <v>11</v>
-      </c>
-      <c r="G112" t="s">
-        <v>11</v>
+      <c r="B112" s="59" t="s">
+        <v>79</v>
+      </c>
+      <c r="C112" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="D112" s="59">
+        <v>3500</v>
+      </c>
+      <c r="E112" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="F112" s="59" t="s">
+        <v>89</v>
+      </c>
+      <c r="G112" s="59">
+        <v>1E-4</v>
       </c>
       <c r="H112" t="s">
         <v>11</v>
@@ -4722,27 +4943,27 @@
         <v>11</v>
       </c>
     </row>
-    <row r="113" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>11</v>
       </c>
-      <c r="B113" t="s">
-        <v>11</v>
-      </c>
-      <c r="C113" t="s">
-        <v>11</v>
-      </c>
-      <c r="D113" t="s">
-        <v>11</v>
-      </c>
-      <c r="E113" t="s">
-        <v>11</v>
-      </c>
-      <c r="F113" t="s">
-        <v>11</v>
-      </c>
-      <c r="G113" t="s">
-        <v>11</v>
+      <c r="B113" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="C113" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="D113" s="59">
+        <v>4000</v>
+      </c>
+      <c r="E113" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="F113" s="59" t="s">
+        <v>89</v>
+      </c>
+      <c r="G113" s="59">
+        <v>1E-4</v>
       </c>
       <c r="H113" t="s">
         <v>11</v>
@@ -4754,27 +4975,27 @@
         <v>11</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>11</v>
       </c>
-      <c r="B114" t="s">
-        <v>11</v>
-      </c>
-      <c r="C114" t="s">
-        <v>11</v>
-      </c>
-      <c r="D114" t="s">
-        <v>11</v>
-      </c>
-      <c r="E114" t="s">
-        <v>11</v>
-      </c>
-      <c r="F114" t="s">
-        <v>11</v>
-      </c>
-      <c r="G114" t="s">
-        <v>11</v>
+      <c r="B114" s="59" t="s">
+        <v>84</v>
+      </c>
+      <c r="C114" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="D114" s="59">
+        <v>4500</v>
+      </c>
+      <c r="E114" s="59" t="s">
+        <v>91</v>
+      </c>
+      <c r="F114" s="59" t="s">
+        <v>89</v>
+      </c>
+      <c r="G114" s="59">
+        <v>1E-4</v>
       </c>
       <c r="H114" t="s">
         <v>11</v>
@@ -4786,28 +5007,10 @@
         <v>11</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>11</v>
       </c>
-      <c r="B115" t="s">
-        <v>11</v>
-      </c>
-      <c r="C115" t="s">
-        <v>11</v>
-      </c>
-      <c r="D115" t="s">
-        <v>11</v>
-      </c>
-      <c r="E115" t="s">
-        <v>11</v>
-      </c>
-      <c r="F115" t="s">
-        <v>11</v>
-      </c>
-      <c r="G115" t="s">
-        <v>11</v>
-      </c>
       <c r="H115" t="s">
         <v>11</v>
       </c>
@@ -4818,28 +5021,18 @@
         <v>11</v>
       </c>
     </row>
-    <row r="116" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>11</v>
       </c>
-      <c r="B116" t="s">
-        <v>11</v>
-      </c>
-      <c r="C116" t="s">
-        <v>11</v>
-      </c>
-      <c r="D116" t="s">
-        <v>11</v>
-      </c>
-      <c r="E116" t="s">
-        <v>11</v>
-      </c>
-      <c r="F116" t="s">
-        <v>11</v>
-      </c>
-      <c r="G116" t="s">
-        <v>11</v>
-      </c>
+      <c r="B116" s="60" t="s">
+        <v>92</v>
+      </c>
+      <c r="C116" s="61"/>
+      <c r="D116" s="61"/>
+      <c r="E116" s="61"/>
+      <c r="F116" s="61"/>
+      <c r="G116" s="61"/>
       <c r="H116" t="s">
         <v>11</v>
       </c>
@@ -4850,27 +5043,27 @@
         <v>11</v>
       </c>
     </row>
-    <row r="117" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>11</v>
       </c>
-      <c r="B117" t="s">
-        <v>11</v>
-      </c>
-      <c r="C117" t="s">
-        <v>11</v>
-      </c>
-      <c r="D117" t="s">
-        <v>11</v>
-      </c>
-      <c r="E117" t="s">
-        <v>11</v>
-      </c>
-      <c r="F117" t="s">
-        <v>11</v>
-      </c>
-      <c r="G117" t="s">
-        <v>11</v>
+      <c r="B117" s="58" t="s">
+        <v>74</v>
+      </c>
+      <c r="C117" s="58" t="s">
+        <v>93</v>
+      </c>
+      <c r="D117" s="58" t="s">
+        <v>94</v>
+      </c>
+      <c r="E117" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="F117" s="58" t="s">
+        <v>96</v>
+      </c>
+      <c r="G117" s="58" t="s">
+        <v>97</v>
       </c>
       <c r="H117" t="s">
         <v>11</v>
@@ -4882,27 +5075,27 @@
         <v>11</v>
       </c>
     </row>
-    <row r="118" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>11</v>
       </c>
-      <c r="B118" t="s">
-        <v>11</v>
-      </c>
-      <c r="C118" t="s">
-        <v>11</v>
-      </c>
-      <c r="D118" t="s">
-        <v>11</v>
-      </c>
-      <c r="E118" t="s">
-        <v>11</v>
-      </c>
-      <c r="F118" t="s">
-        <v>11</v>
-      </c>
-      <c r="G118" t="s">
-        <v>11</v>
+      <c r="B118" s="59" t="s">
+        <v>98</v>
+      </c>
+      <c r="C118" s="59" t="s">
+        <v>99</v>
+      </c>
+      <c r="D118" s="59" t="s">
+        <v>100</v>
+      </c>
+      <c r="E118" s="59" t="s">
+        <v>101</v>
+      </c>
+      <c r="F118" s="59" t="s">
+        <v>27</v>
+      </c>
+      <c r="G118" s="62">
+        <v>30000</v>
       </c>
       <c r="H118" t="s">
         <v>11</v>
@@ -4914,27 +5107,27 @@
         <v>11</v>
       </c>
     </row>
-    <row r="119" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>11</v>
       </c>
-      <c r="B119" t="s">
-        <v>11</v>
-      </c>
-      <c r="C119" t="s">
-        <v>11</v>
-      </c>
-      <c r="D119" t="s">
-        <v>11</v>
-      </c>
-      <c r="E119" t="s">
-        <v>11</v>
-      </c>
-      <c r="F119" t="s">
-        <v>11</v>
-      </c>
-      <c r="G119" t="s">
-        <v>11</v>
+      <c r="B119" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="C119" s="59" t="s">
+        <v>103</v>
+      </c>
+      <c r="D119" s="59" t="s">
+        <v>104</v>
+      </c>
+      <c r="E119" s="59" t="s">
+        <v>105</v>
+      </c>
+      <c r="F119" s="59" t="s">
+        <v>27</v>
+      </c>
+      <c r="G119" s="62">
+        <v>35000</v>
       </c>
       <c r="H119" t="s">
         <v>11</v>
@@ -4946,27 +5139,27 @@
         <v>11</v>
       </c>
     </row>
-    <row r="120" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>11</v>
       </c>
-      <c r="B120" t="s">
-        <v>11</v>
-      </c>
-      <c r="C120" t="s">
-        <v>11</v>
-      </c>
-      <c r="D120" t="s">
-        <v>11</v>
-      </c>
-      <c r="E120" t="s">
-        <v>11</v>
-      </c>
-      <c r="F120" t="s">
-        <v>11</v>
-      </c>
-      <c r="G120" t="s">
-        <v>11</v>
+      <c r="B120" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="C120" s="59" t="s">
+        <v>107</v>
+      </c>
+      <c r="D120" s="59" t="s">
+        <v>108</v>
+      </c>
+      <c r="E120" s="59" t="s">
+        <v>109</v>
+      </c>
+      <c r="F120" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="G120" s="62">
+        <v>55000</v>
       </c>
       <c r="H120" t="s">
         <v>11</v>
@@ -4978,10 +5171,146 @@
         <v>11</v>
       </c>
     </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B122" s="60" t="s">
+        <v>110</v>
+      </c>
+      <c r="C122" s="61"/>
+      <c r="D122" s="61"/>
+      <c r="E122" s="61"/>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B123" s="58" t="s">
+        <v>74</v>
+      </c>
+      <c r="C123" s="58" t="s">
+        <v>75</v>
+      </c>
+      <c r="D123" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="E123" s="58" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B124" s="59" t="s">
+        <v>98</v>
+      </c>
+      <c r="C124" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="D124" s="59">
+        <v>1</v>
+      </c>
+      <c r="E124" s="59" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B125" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="C125" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="D125" s="59">
+        <v>1.5</v>
+      </c>
+      <c r="E125" s="59" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B126" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="C126" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="D126" s="59">
+        <v>2</v>
+      </c>
+      <c r="E126" s="59" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B128" s="60" t="s">
+        <v>112</v>
+      </c>
+      <c r="C128" s="61"/>
+      <c r="D128" s="61"/>
+      <c r="E128" s="61"/>
+    </row>
+    <row r="129" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B129" s="58" t="s">
+        <v>74</v>
+      </c>
+      <c r="C129" s="58" t="s">
+        <v>75</v>
+      </c>
+      <c r="D129" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="E129" s="58" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="130" spans="2:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B130" s="59" t="s">
+        <v>98</v>
+      </c>
+      <c r="C130" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="D130" s="59">
+        <v>3</v>
+      </c>
+      <c r="E130" s="59" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="131" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B131" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="C131" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="D131" s="59">
+        <v>3</v>
+      </c>
+      <c r="E131" s="59" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="132" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B132" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="C132" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="D132" s="59">
+        <v>1</v>
+      </c>
+      <c r="E132" s="59" t="s">
+        <v>115</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B104:F104"/>
+    <mergeCell ref="B110:G110"/>
+    <mergeCell ref="B116:G116"/>
+    <mergeCell ref="B122:E122"/>
+    <mergeCell ref="B128:E128"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:J2 A49:J49 F48:J48 A41:J43 G40:J40 A35:J39 I34:J34 A28:J33 A26 I26:J27 A13:J16 J12 A7:J11 J6 A63:J67 I62:J62 A69:J88 I68:J68 A91:J95 A89 A5:J5 A4 D4 A3:D3 F3:J3 F4:J4 A19:J25 A17:C18 E17:J18 A46:J47 A44:B44 D44:J44 A45:C45 E45:J45 A53 A50 D50:J50 A51 C51 A52:B52 D52:J52 A55:J55 A54:B54 D54:J54 C53 E53:J53 E51:J51 A57:J61 E56:J56 A97:J120 A96 A90:I90" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:J2 A49:J49 F48:J48 A41:J43 G40:J40 A35:J39 I34:J34 A28:J33 A26 I26:J27 A13:J16 J12 A7:J11 J6 A63:J67 I62:J62 A69:J88 I68:J68 A91:J95 A89 A5:J5 A4 D4 A3:D3 F3:J3 F4:J4 A19:J25 A17:C18 E17:J18 A46:J47 A44:B44 D44:J44 A45:C45 E45:J45 A53 A50 D50:J50 A51 C51 A52:B52 D52:J52 A55:J55 A54:B54 D54:J54 C53 E53:J53 E51:J51 A57:J61 E56:J56 A97:J103 A96 A90:I90 A104:A120 H104:J120" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>